<commit_message>
was refactored class merge functionality
</commit_message>
<xml_diff>
--- a/output/revenue_template_v1final31.xlsx
+++ b/output/revenue_template_v1final31.xlsx
@@ -680,10 +680,10 @@
     <t>Bench</t>
   </si>
   <si>
+    <t>Oleg Dudar</t>
+  </si>
+  <si>
     <t>Nazar Khimin</t>
-  </si>
-  <si>
-    <t>Oleg Dudar</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -14160,10 +14160,10 @@
         <v>217</v>
       </c>
       <c r="B89" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="K89" t="s" s="1829">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="L89">
         <f>IF(+K89=T3,W3,IF(K89=T4,W4,if(K89=T5,W5,if(K89=T6,W6,if(K89=T7,W7)))))</f>
@@ -14174,10 +14174,10 @@
         <v>217</v>
       </c>
       <c r="B90" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="K90" t="s" s="1831">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="L90">
         <f>IF(+K90=T3,W3,IF(K90=T4,W4,if(K90=T5,W5,if(K90=T6,W6,if(K90=T7,W7)))))</f>
@@ -14188,10 +14188,10 @@
         <v>217</v>
       </c>
       <c r="B91" t="s">
-        <v>218</v>
+        <v>76</v>
       </c>
       <c r="K91" t="s" s="1833">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L91">
         <f>IF(+K91=T3,W3,IF(K91=T4,W4,if(K91=T5,W5,if(K91=T6,W6,if(K91=T7,W7)))))</f>
@@ -14205,7 +14205,7 @@
         <v>219</v>
       </c>
       <c r="K92" t="s" s="1835">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L92">
         <f>IF(+K92=T3,W3,IF(K92=T4,W4,if(K92=T5,W5,if(K92=T6,W6,if(K92=T7,W7)))))</f>

</xml_diff>